<commit_message>
new data from production guides
</commit_message>
<xml_diff>
--- a/src/data/roteiro.xlsx
+++ b/src/data/roteiro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.rossi\Documents\quasar\lean-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2DB13F-9B79-4D79-81F4-76BA583DED86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD5739A-CDB5-4F03-95CF-055225B569E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{79507F9C-91F9-4D15-AB37-7A21D05358D7}"/>
   </bookViews>
@@ -1516,7 +1516,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>